<commit_message>
Added a new attribute agenteMaritimo
</commit_message>
<xml_diff>
--- a/files/Anexo_5532893_Porto_sem_papel_amostragem.xlsx
+++ b/files/Anexo_5532893_Porto_sem_papel_amostragem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.catossi\source\repos\zwt-api\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E277498F-F345-4C83-A9A2-4AFFBE896946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F2AD06-AA00-46BD-B3A9-438E808ADE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4D563B2B-388C-48B9-B4AC-3B7E61F16DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D563B2B-388C-48B9-B4AC-3B7E61F16DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="tb_agencias" sheetId="1" r:id="rId1"/>
@@ -4056,11 +4056,11 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15196,7 +15196,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18869,12 +18869,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1301</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19425,7 +19425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D5490F-AE1A-40FA-BFB0-7403022990A7}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -19623,7 +19623,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F15" s="9"/>
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -19634,7 +19634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D177E53-C599-48BC-8CCA-1E379662C7BC}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>